<commit_message>
Updated M3406 Part Number for BOM
Old part number is discontinued
</commit_message>
<xml_diff>
--- a/000-1St Anniversary SP/BOM_CK_Ann_SP.xlsx
+++ b/000-1St Anniversary SP/BOM_CK_Ann_SP.xlsx
@@ -1,12 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet sheetId="1" name="BOM_BNO085_Ann_Choco_ANN_2024-0" state="visible" r:id="rId4"/>
+    <sheet state="visible" name="BOM_BNO085_Ann_Choco_ANN_2024-0" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <definedNames/>
+  <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="MOXwmYPISTzrG24T+YpoYBJKWFW77SuQ8XtfMZ8Bf6s="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -421,7 +426,7 @@
     <t>西安航天民芯</t>
   </si>
   <si>
-    <t>C83224</t>
+    <t>C22462728</t>
   </si>
   <si>
     <t>23</t>
@@ -499,14 +504,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="2">
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <color theme="1"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -514,55 +523,50 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="4F81BD"/>
@@ -586,79 +590,19 @@
         <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="0000FF"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -670,1087 +614,1997 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col customWidth="1" min="1" max="10" width="20.0"/>
+    <col customWidth="1" min="11" max="26" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6">
+      <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12">
+      <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15">
+      <c r="A15" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16">
+      <c r="A16" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17">
+      <c r="A17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18">
+      <c r="A18" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19">
+      <c r="A19" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20">
+      <c r="A20" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions gridLines="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>